<commit_message>
Added the maps I could for starters
</commit_message>
<xml_diff>
--- a/Data/City_Stats.xlsx
+++ b/Data/City_Stats.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA2692F-B994-4511-A83D-9B24F8134A50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="32400" yWindow="0" windowWidth="15300" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Boston_MA</t>
   </si>
@@ -51,25 +52,34 @@
     <t>Washington_DC</t>
   </si>
   <si>
-    <t>Index</t>
-  </si>
-  <si>
-    <t>Zscore</t>
-  </si>
-  <si>
-    <t>Pvalue</t>
-  </si>
-  <si>
     <t>Dist_Mean</t>
   </si>
   <si>
     <t>HLTH_Mean</t>
+  </si>
+  <si>
+    <t>Health_Index</t>
+  </si>
+  <si>
+    <t>Health_Zscore</t>
+  </si>
+  <si>
+    <t>Health_Pvalue</t>
+  </si>
+  <si>
+    <t>Comb_Index</t>
+  </si>
+  <si>
+    <t>Comb_Zscore</t>
+  </si>
+  <si>
+    <t>Comb_Pvalue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,36 +390,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -420,12 +447,12 @@
         <v>1.231214</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -445,7 +472,7 @@
         <v>1.2431509999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -465,7 +492,7 @@
         <v>1.24183</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -485,7 +512,7 @@
         <v>1.241573</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -505,7 +532,7 @@
         <v>1.24359</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -525,7 +552,7 @@
         <v>1.236111</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -539,7 +566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -553,7 +580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Here are my maps boo
</commit_message>
<xml_diff>
--- a/Data/City_Stats.xlsx
+++ b/Data/City_Stats.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA2692F-B994-4511-A83D-9B24F8134A50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="32400" yWindow="0" windowWidth="15300" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32400" yWindow="0" windowWidth="15300" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -390,11 +389,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,17 +439,59 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>0.190191</v>
+      </c>
+      <c r="C2">
+        <v>15.499238999999999</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2">
         <v>2.6936420000000001</v>
       </c>
       <c r="F2">
         <v>1.231214</v>
+      </c>
+      <c r="G2">
+        <v>0.17596400000000001</v>
+      </c>
+      <c r="H2">
+        <v>14.390506</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>0.14471800000000001</v>
+      </c>
+      <c r="C3">
+        <v>12.434471</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>2.4265729999999999</v>
+      </c>
+      <c r="F3">
+        <v>1.2412589999999999</v>
+      </c>
+      <c r="G3">
+        <v>8.9472999999999997E-2</v>
+      </c>
+      <c r="H3">
+        <v>7.9266959999999997</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -471,6 +512,15 @@
       <c r="F4">
         <v>1.2431509999999999</v>
       </c>
+      <c r="G4">
+        <v>0.25911099999999998</v>
+      </c>
+      <c r="H4">
+        <v>7.3843180000000004</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -491,6 +541,15 @@
       <c r="F5">
         <v>1.24183</v>
       </c>
+      <c r="G5">
+        <v>0.62871500000000002</v>
+      </c>
+      <c r="H5">
+        <v>18.56551</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -510,6 +569,15 @@
       </c>
       <c r="F6">
         <v>1.241573</v>
+      </c>
+      <c r="G6">
+        <v>0.23713699999999999</v>
+      </c>
+      <c r="H6">
+        <v>12.060738000000001</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>